<commit_message>
fix: images . feat: add site map
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO (1).xlsx
+++ b/Modèle-audit-SEO (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="7520" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="7660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>Catégorie</t>
   </si>
@@ -40,52 +40,162 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>Titre de la page</t>
+    <t>Titre des pages</t>
+  </si>
+  <si>
+    <t>Le titre de la page principale est "." et celui de la page contact est "page 2"</t>
   </si>
   <si>
     <t>Choisir un titre adapté au contenu</t>
   </si>
   <si>
-    <t>Changer de titre</t>
-  </si>
-  <si>
-    <t>Nom de la page contact</t>
-  </si>
-  <si>
-    <t>Responsive header page contact</t>
-  </si>
-  <si>
-    <t>Les paragraphes sont des images</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Le code de la page contact n'est pas correctement relié avec le css, le javascript et les frameworks</t>
+  </si>
+  <si>
+    <t>La page contact n'est donc pas responsive ce qui va, d'une part augmenter le taux de rebond des utilisateurs et poser un problème de SEO</t>
+  </si>
+  <si>
+    <t>Lier correctement les codes</t>
+  </si>
+  <si>
+    <t>Certains paragraphes sont des images</t>
+  </si>
+  <si>
+    <t>Pose problème au niveau du responsive du site, et empèche l'utilisation de mots clés</t>
+  </si>
+  <si>
+    <t>Remplacer les images par du texte, et utiliser des balises &lt;strong&gt; pour les mots clés</t>
   </si>
   <si>
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Ajouter du padding sur les icônes</t>
-  </si>
-  <si>
     <t>Taille de police</t>
   </si>
   <si>
-    <t>Couleur du bloc</t>
-  </si>
-  <si>
-    <t>Taille des photos</t>
-  </si>
-  <si>
-    <t>Liens annuaires</t>
-  </si>
-  <si>
-    <t>Pas d'évoquation de l'adresse</t>
-  </si>
-  <si>
-    <t>&lt;link rel href=lang&gt;</t>
-  </si>
-  <si>
-    <t>Code trop lourd</t>
+    <t>La taille de la police est trop petite, et donc difficilement lisible</t>
+  </si>
+  <si>
+    <t>Augmenter la taille du texte et utiliser des valeurs de taille relatives au lieu de valeurs absolues afin d'améliorer l'accessibilité du site. ("rem" au lieu de "px")</t>
+  </si>
+  <si>
+    <t>Ratio de contraste des couleurs trop faible</t>
+  </si>
+  <si>
+    <t>La lisibilité de certains éléments est compromise par un manque de contraste entre l'arrière plan et le texte. Le contraste entre le fond et le texte doit être de 3:1 pour les titres et 4,5:1 pour les paragraphes</t>
+  </si>
+  <si>
+    <t>Augmenter les contrastes en changeant d'arrière plan 
+ou la couleur des textes</t>
+  </si>
+  <si>
+    <t>La taille et le format des photos utilisés</t>
+  </si>
+  <si>
+    <t>La taille des photographies n'est pas adaptée 
+à la taille des écrans, et le format de celles-ci n'est pas adapté à une utilisation web. Ce qui va avoir pour résultat d'alourdir le site et augmenter le temps de chargement des pages</t>
+  </si>
+  <si>
+    <t>Réduire la taille des photos et les compresser.</t>
+  </si>
+  <si>
+    <t>Liens dans le footer</t>
+  </si>
+  <si>
+    <t>Trop de liens inutiles dans le seul but d'augmenter classement SEO et tromper Gooogle. Pratique consiérée comme du "black hat"</t>
+  </si>
+  <si>
+    <t>Supprimer les liens inutiles.</t>
+  </si>
+  <si>
+    <t>Evocation de l'adresse quasiment invisible</t>
+  </si>
+  <si>
+    <t>En visitant le site, l'utilisateur peux passer à côté du fait que l'entreprise a une existence physique</t>
+  </si>
+  <si>
+    <t>Créer une page Google MyBuisiness,  et implémenter une carte dans le site</t>
+  </si>
+  <si>
+    <t>Langue non indiquée dans le code HTML</t>
+  </si>
+  <si>
+    <t>Dans la partie head du code HTML la langue est definie comme "default", ce qui ne donne aucune information sur la langue utilisée</t>
+  </si>
+  <si>
+    <t>Changer la langue pour "fr"</t>
+  </si>
+  <si>
+    <t>Code source trop lourd</t>
+  </si>
+  <si>
+    <t>Import des librairies complètes de bootstrap et Jquery</t>
   </si>
   <si>
     <t>Pas de balises sémantiques (div only)</t>
+  </si>
+  <si>
+    <t>Le code HTML n'utilise quasiment aucune balise sémantique, ce qui rend le code difficilement lisible par les robots ainsi que les développeurs</t>
+  </si>
+  <si>
+    <t>Ajouter des balises comme:  &lt;header&gt;, &lt;main&gt;, &lt;section&gt; etc...</t>
+  </si>
+  <si>
+    <t>Texte alternatif des images</t>
+  </si>
+  <si>
+    <t>Les textes situés dans les "alt" sont des mots clés, et non une description des images. Ce qui n'a aucune utilité au niveau du SEO, et nuit gravement à l'accessibilité du site</t>
+  </si>
+  <si>
+    <t>Ecrire un texte qui décrit les images</t>
+  </si>
+  <si>
+    <t>Le site n'a pas de description</t>
+  </si>
+  <si>
+    <t>La balise &lt;meta description&gt; n'a pas de contenu, ce qui va poser un problème pour les utilisateurs et le référencement du site</t>
+  </si>
+  <si>
+    <t>Ecrire une description pour le site.</t>
+  </si>
+  <si>
+    <t>Du texte caché est disséminé partout dans le site</t>
+  </si>
+  <si>
+    <t>Des mots clés transparents sont disséminés partout à travers le site. Les robots de google risquent de sanctionnerle référencement du site pour pratique frauduleuse "black hat"</t>
+  </si>
+  <si>
+    <t>Supprimer les textes cachés</t>
+  </si>
+  <si>
+    <t>Pas de largeur maximale definie pour le site</t>
+  </si>
+  <si>
+    <t>Les backgrounds du site s'étendent à l'infini</t>
+  </si>
+  <si>
+    <t>Definir une taille maximale pour le site</t>
+  </si>
+  <si>
+    <t>Le site n'est pas suivi par Google Analytics et Google Search Console</t>
+  </si>
+  <si>
+    <t>Les champs prévus à cet effet ne sont pas remplis</t>
+  </si>
+  <si>
+    <t>Le suivi de la fréquentation du site aidera à identifier les problèmes de référencements et les possibilités d'améliorations</t>
+  </si>
+  <si>
+    <t>Les pages ne sont pas indexés sur Google</t>
+  </si>
+  <si>
+    <t>Les balises ne sont pas existantes pour l'indexation du site par Google</t>
+  </si>
+  <si>
+    <t>Création d'une &lt;meta&gt; "robot" ainsi que d'une &lt;meta&gt; "canonical"</t>
   </si>
 </sst>
 </file>
@@ -93,12 +203,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +236,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -147,20 +264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -169,6 +272,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -178,9 +302,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,6 +324,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -231,7 +362,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,15 +376,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,20 +392,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -297,187 +414,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,6 +680,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -577,173 +705,174 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,17 +1132,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2846153846154" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.6153846153846" customWidth="1"/>
-    <col min="2" max="2" width="32.1538461538462" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="2" max="2" width="44.6153846153846" customWidth="1"/>
+    <col min="3" max="3" width="41.3461538461538" customWidth="1"/>
     <col min="4" max="4" width="30.7692307692308" customWidth="1"/>
     <col min="5" max="5" width="22.0769230769231" customWidth="1"/>
     <col min="6" max="6" width="21.2846153846154" customWidth="1"/>
@@ -1021,182 +1150,342 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" ht="45" customHeight="1" spans="1:6">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A4" t="s">
+    <row r="4" ht="49" customHeight="1" spans="1:6">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="F4" s="6"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A5" t="s">
+    <row r="5" ht="54" customHeight="1" spans="1:6">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A6" t="s">
+    <row r="6" ht="88" customHeight="1" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" ht="99" customHeight="1" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" ht="77" customHeight="1" spans="1:6">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4"/>
+    <row r="9" ht="67" customHeight="1" spans="1:6">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4"/>
+    <row r="10" ht="48" customHeight="1" spans="1:6">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4"/>
+    <row r="11" ht="60" customHeight="1" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A10" t="s">
+    <row r="12" ht="58" customHeight="1" spans="1:6">
+      <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" ht="63" customHeight="1" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" ht="70" customHeight="1" spans="1:6">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="6"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A11" t="s">
+    <row r="15" ht="59" customHeight="1" spans="1:6">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A12" t="s">
+    <row r="16" ht="67" customHeight="1" spans="1:5">
+      <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A13" t="s">
+    <row r="17" ht="66" customHeight="1" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" ht="68" customHeight="1" spans="1:5">
+      <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A14" t="s">
+    <row r="19" s="1" customFormat="1" ht="64" customHeight="1" spans="1:5">
+      <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="4"/>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -2176,8 +2465,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>

</xml_diff>